<commit_message>
Implementación de formulario de disponibilidad y formulario PIR para las regiones.
</commit_message>
<xml_diff>
--- a/public/templates/ausencias.xlsx
+++ b/public/templates/ausencias.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="792" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="792"/>
   </bookViews>
   <sheets>
     <sheet name="Ausencias" sheetId="6" r:id="rId1"/>
@@ -883,36 +883,36 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1882,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K25"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1900,28 +1900,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" ht="18.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
     </row>
     <row r="4" spans="1:11" ht="18.75">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:11" ht="18.75">
       <c r="A5" s="7"/>
@@ -2013,13 +2013,13 @@
     <row r="11" spans="1:11">
       <c r="A11" s="26"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="26"/>
@@ -2031,10 +2031,10 @@
       <c r="E12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="6"/>
@@ -2083,14 +2083,14 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
     </row>
     <row r="18" spans="1:3" ht="15.75">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" s="8"/>
@@ -2147,7 +2147,7 @@
   <dimension ref="A3:K25"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2164,28 +2164,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" ht="18.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
     </row>
     <row r="4" spans="1:11" ht="18.75">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:11" ht="18.75">
       <c r="A5" s="40"/>
@@ -2277,13 +2277,13 @@
     <row r="11" spans="1:11">
       <c r="A11" s="26"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="26"/>
@@ -2295,10 +2295,10 @@
       <c r="E12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="6"/>
@@ -2347,14 +2347,14 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
     </row>
     <row r="18" spans="1:3" ht="15.75">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" s="39"/>
@@ -2410,8 +2410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H4"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2428,28 +2428,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:11" ht="18.75">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
     </row>
     <row r="4" spans="1:11" ht="18.75">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:11" ht="18.75">
       <c r="A5" s="40"/>
@@ -2541,13 +2541,13 @@
     <row r="11" spans="1:11">
       <c r="A11" s="26"/>
       <c r="B11" s="25"/>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="26"/>
@@ -2559,10 +2559,10 @@
       <c r="E12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="45"/>
+      <c r="G12" s="48"/>
     </row>
     <row r="13" spans="1:11">
       <c r="B13" s="6"/>
@@ -2611,14 +2611,14 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="43"/>
     </row>
     <row r="18" spans="1:3" ht="15.75">
-      <c r="A18" s="52"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
     </row>
     <row r="19" spans="1:3" ht="15.75">
       <c r="A19" s="39"/>
@@ -2684,74 +2684,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="47"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="47" t="s">
+      <c r="A8" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
     </row>
     <row r="10" spans="1:3" ht="15.75">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="48"/>
-      <c r="C10" s="48"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>